<commit_message>
Cleaned up and updated "card" and "player" Excel and SQL files.
</commit_message>
<xml_diff>
--- a/cardshifter-database/cardshifter-0.4-card-list.xlsx
+++ b/cardshifter-database/cardshifter-0.4-card-list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3820" yWindow="0" windowWidth="21660" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="item.csv" sheetId="1" r:id="rId1"/>
@@ -290,23 +290,7 @@
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
@@ -633,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S30"/>
+  <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S32" sqref="S32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -668,8 +652,8 @@
     </row>
     <row r="2" spans="1:19">
       <c r="S2" s="6" t="str">
-        <f xml:space="preserve"> "SET SEARCH_PATH TO cardshifter_stats; DELETE FROM card;"</f>
-        <v>SET SEARCH_PATH TO cardshifter_stats; DELETE FROM card;</v>
+        <f xml:space="preserve"> "START TRANSACTION; SET SEARCH_PATH TO cardshifter_stats; DELETE FROM card;"</f>
+        <v>START TRANSACTION; SET SEARCH_PATH TO cardshifter_stats; DELETE FROM card;</v>
       </c>
     </row>
     <row r="3" spans="1:19" s="3" customFormat="1">
@@ -850,7 +834,7 @@
         <v>1</v>
       </c>
       <c r="S5" s="6" t="str">
-        <f t="shared" ref="S5:S30" si="1" xml:space="preserve"> "("&amp;A5&amp;","&amp;B5&amp;","&amp;C5&amp;","&amp;D5&amp;","&amp;E5&amp;","&amp;F5&amp;","&amp;H5&amp;","&amp;J5&amp;","&amp;L5&amp;","&amp;N5&amp;","&amp;P5&amp;","&amp;Q5&amp;","&amp;R5&amp;"),"</f>
+        <f t="shared" ref="S5:S29" si="1" xml:space="preserve"> "("&amp;A5&amp;","&amp;B5&amp;","&amp;C5&amp;","&amp;D5&amp;","&amp;E5&amp;","&amp;F5&amp;","&amp;H5&amp;","&amp;J5&amp;","&amp;L5&amp;","&amp;N5&amp;","&amp;P5&amp;","&amp;Q5&amp;","&amp;R5&amp;"),"</f>
         <v>(2,1,null,null,null,'B0T',1,1,1,null,1,1,1),</v>
       </c>
     </row>
@@ -2370,9 +2354,14 @@
         <v>(27,1,null,null,null,null,3,3,null,5,null,null,null);</v>
       </c>
     </row>
+    <row r="31" spans="1:19">
+      <c r="S31" s="6" t="str">
+        <f>"COMMIT;"</f>
+        <v>COMMIT;</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Improved database schema, added 'Enhancement' card type.
</commit_message>
<xml_diff>
--- a/cardshifter-database/cardshifter-0.4-card-list.xlsx
+++ b/cardshifter-database/cardshifter-0.4-card-list.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="14">
   <si>
     <t>type</t>
   </si>
@@ -619,15 +619,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S32" sqref="S32"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="4" width="10.83203125" style="1"/>
     <col min="5" max="5" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -1830,8 +1830,9 @@
       <c r="E22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>11</v>
+      <c r="F22" s="1" t="str">
+        <f>"'Enhancement'"</f>
+        <v>'Enhancement'</v>
       </c>
       <c r="G22" s="1">
         <v>1</v>
@@ -1871,7 +1872,7 @@
       </c>
       <c r="S22" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>(19,1,null,null,null,null,2,0,null,1,null,null,null),</v>
+        <v>(19,1,null,null,null,'Enhancement',2,0,null,1,null,null,null),</v>
       </c>
     </row>
     <row r="23" spans="1:19">
@@ -1890,8 +1891,9 @@
       <c r="E23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>11</v>
+      <c r="F23" s="1" t="str">
+        <f t="shared" ref="F23:F30" si="3">"'Enhancement'"</f>
+        <v>'Enhancement'</v>
       </c>
       <c r="G23" s="1">
         <v>0</v>
@@ -1931,7 +1933,7 @@
       </c>
       <c r="S23" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>(20,1,null,null,null,null,0,2,null,1,null,null,null),</v>
+        <v>(20,1,null,null,null,'Enhancement',0,2,null,1,null,null,null),</v>
       </c>
     </row>
     <row r="24" spans="1:19">
@@ -1950,8 +1952,9 @@
       <c r="E24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>11</v>
+      <c r="F24" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>'Enhancement'</v>
       </c>
       <c r="G24" s="1">
         <v>1</v>
@@ -1991,7 +1994,7 @@
       </c>
       <c r="S24" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>(21,1,null,null,null,null,1,1,null,1,null,null,null),</v>
+        <v>(21,1,null,null,null,'Enhancement',1,1,null,1,null,null,null),</v>
       </c>
     </row>
     <row r="25" spans="1:19">
@@ -2010,8 +2013,9 @@
       <c r="E25" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>11</v>
+      <c r="F25" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>'Enhancement'</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>11</v>
@@ -2051,7 +2055,7 @@
       </c>
       <c r="S25" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>(22,1,null,null,null,null,1,2,null,2,null,null,null),</v>
+        <v>(22,1,null,null,null,'Enhancement',1,2,null,2,null,null,null),</v>
       </c>
     </row>
     <row r="26" spans="1:19">
@@ -2070,8 +2074,9 @@
       <c r="E26" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>11</v>
+      <c r="F26" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>'Enhancement'</v>
       </c>
       <c r="G26" s="1">
         <v>2</v>
@@ -2111,7 +2116,7 @@
       </c>
       <c r="S26" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>(23,1,null,null,null,null,2,1,null,2,null,null,null),</v>
+        <v>(23,1,null,null,null,'Enhancement',2,1,null,2,null,null,null),</v>
       </c>
     </row>
     <row r="27" spans="1:19">
@@ -2130,8 +2135,9 @@
       <c r="E27" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>11</v>
+      <c r="F27" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>'Enhancement'</v>
       </c>
       <c r="G27" s="1">
         <v>3</v>
@@ -2171,7 +2177,7 @@
       </c>
       <c r="S27" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>(24,1,null,null,null,null,3,0,null,2,null,null,null),</v>
+        <v>(24,1,null,null,null,'Enhancement',3,0,null,2,null,null,null),</v>
       </c>
     </row>
     <row r="28" spans="1:19">
@@ -2190,8 +2196,9 @@
       <c r="E28" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>11</v>
+      <c r="F28" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>'Enhancement'</v>
       </c>
       <c r="G28" s="1">
         <v>0</v>
@@ -2231,7 +2238,7 @@
       </c>
       <c r="S28" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>(25,1,null,null,null,null,0,3,null,2,null,null,null),</v>
+        <v>(25,1,null,null,null,'Enhancement',0,3,null,2,null,null,null),</v>
       </c>
     </row>
     <row r="29" spans="1:19">
@@ -2250,8 +2257,9 @@
       <c r="E29" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>11</v>
+      <c r="F29" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>'Enhancement'</v>
       </c>
       <c r="G29" s="1">
         <v>2</v>
@@ -2291,7 +2299,7 @@
       </c>
       <c r="S29" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>(26,1,null,null,null,null,2,2,null,3,null,null,null),</v>
+        <v>(26,1,null,null,null,'Enhancement',2,2,null,3,null,null,null),</v>
       </c>
     </row>
     <row r="30" spans="1:19">
@@ -2310,8 +2318,9 @@
       <c r="E30" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>11</v>
+      <c r="F30" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>'Enhancement'</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>11</v>
@@ -2351,7 +2360,7 @@
       </c>
       <c r="S30" s="6" t="str">
         <f xml:space="preserve"> "("&amp;A30&amp;","&amp;B30&amp;","&amp;C30&amp;","&amp;D30&amp;","&amp;E30&amp;","&amp;F30&amp;","&amp;H30&amp;","&amp;J30&amp;","&amp;L30&amp;","&amp;N30&amp;","&amp;P30&amp;","&amp;Q30&amp;","&amp;R30&amp;");"</f>
-        <v>(27,1,null,null,null,null,3,3,null,5,null,null,null);</v>
+        <v>(27,1,null,null,null,'Enhancement',3,3,null,5,null,null,null);</v>
       </c>
     </row>
     <row r="31" spans="1:19">

</xml_diff>